<commit_message>
Update with Karasjok site
</commit_message>
<xml_diff>
--- a/output/permit_maps/permits_sept2021_all_sites.xlsx
+++ b/output/permit_maps/permits_sept2021_all_sites.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Benoit_D\QUANTOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC33F64C-8BAE-495C-AA4A-57710A970F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBDFAA6-933B-442C-9A83-778E44435104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{08867272-A7A1-46A2-B589-C320F206F8A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="permits_sept2021_all_sites" localSheetId="0">Sheet1!$B$1:$H$10</definedName>
+    <definedName name="permits_sept2021_all_sites" localSheetId="0">Sheet1!$B$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{68FAD65E-D74F-4FF1-A05A-DAD40DDB7B52}" name="permits_sept2021_all_sites" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{33F259D6-7C8E-4951-BF2D-339E35117786}" name="permits_sept2021_all_sites1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\JES\Downloads\permits_sept2021_all_sites.csv" thousands=" " tab="0" comma="1">
       <textFields count="13">
         <textField type="skip"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Njahkajavri</t>
   </si>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="permits_sept2021_all_sites" connectionId="1" xr16:uid="{490BBC70-57A3-4BEA-BEB8-62D09077B147}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="permits_sept2021_all_sites" connectionId="1" xr16:uid="{F95646C6-986C-42A4-A718-475D42810F75}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6CADA4-03D9-4692-B062-F0677E2F37E4}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A71387-655C-4309-8AEA-5327D277D28C}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H11" sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -502,7 +502,7 @@
     <col min="3" max="4" width="10.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.73046875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -640,19 +640,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>24.959788799999998</v>
+        <v>25.386399999999998</v>
       </c>
       <c r="D6" s="3">
-        <v>69.609377800000004</v>
+        <v>69.444800000000001</v>
       </c>
       <c r="E6" s="5">
-        <v>420679.50224939297</v>
+        <v>436777.59009725502</v>
       </c>
       <c r="F6" s="5">
-        <v>7723636.85243537</v>
+        <v>7704794.2822894901</v>
       </c>
       <c r="G6">
         <v>35</v>
@@ -666,25 +666,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>25.926961299999999</v>
+        <v>24.959788799999998</v>
       </c>
       <c r="D7" s="3">
-        <v>69.876856700000005</v>
+        <v>69.609377800000004</v>
       </c>
       <c r="E7" s="5">
-        <v>458801.013035307</v>
+        <v>420679.50224939297</v>
       </c>
       <c r="F7" s="5">
-        <v>7752502.8620786304</v>
+        <v>7723636.85243537</v>
       </c>
       <c r="G7">
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
@@ -692,19 +692,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3">
-        <v>26.9157929</v>
+        <v>25.926961299999999</v>
       </c>
       <c r="D8" s="3">
-        <v>69.964763300000001</v>
+        <v>69.876856700000005</v>
       </c>
       <c r="E8" s="5">
-        <v>496780.28296250699</v>
+        <v>458801.013035307</v>
       </c>
       <c r="F8" s="5">
-        <v>7761945.8609598503</v>
+        <v>7752502.8620786304</v>
       </c>
       <c r="G8">
         <v>35</v>
@@ -718,19 +718,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3">
-        <v>26.077548499999999</v>
+        <v>26.9157929</v>
       </c>
       <c r="D9" s="3">
-        <v>69.965256199999999</v>
+        <v>69.964763300000001</v>
       </c>
       <c r="E9" s="5">
-        <v>464731.41287877999</v>
+        <v>496780.28296250699</v>
       </c>
       <c r="F9" s="5">
-        <v>7762265.3401231701</v>
+        <v>7761945.8609598503</v>
       </c>
       <c r="G9">
         <v>35</v>
@@ -744,24 +744,50 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>26.077548499999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>69.965256199999999</v>
+      </c>
+      <c r="E10" s="5">
+        <v>464731.41287877999</v>
+      </c>
+      <c r="F10" s="5">
+        <v>7762265.3401231701</v>
+      </c>
+      <c r="G10">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>27.615827299999999</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>70.140607500000002</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="5">
         <v>523348.12038186798</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F11" s="5">
         <v>7781671.4575946797</v>
       </c>
-      <c r="G10">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G11">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update maps for Helitrans co-ords
</commit_message>
<xml_diff>
--- a/output/permit_maps/permits_sept2021_all_sites.xlsx
+++ b/output/permit_maps/permits_sept2021_all_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBDFAA6-933B-442C-9A83-778E44435104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A53C0-C842-4AF7-BBFD-067FC4A4D30E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{08867272-A7A1-46A2-B589-C320F206F8A7}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Njahkajavri</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Kommune</t>
+  </si>
+  <si>
+    <t>Karasjok Camping</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="A1:H11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -640,19 +643,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>25.386399999999998</v>
+        <v>25.487036705017001</v>
       </c>
       <c r="D6" s="3">
-        <v>69.444800000000001</v>
+        <v>69.467986997867399</v>
       </c>
       <c r="E6" s="5">
-        <v>436777.59009725502</v>
+        <v>440783.85183459503</v>
       </c>
       <c r="F6" s="5">
-        <v>7704794.2822894901</v>
+        <v>7707278.4545117402</v>
       </c>
       <c r="G6">
         <v>35</v>

</xml_diff>